<commit_message>
Added Docket and newsagent
</commit_message>
<xml_diff>
--- a/User Story(2).xlsx
+++ b/User Story(2).xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Documents\GitHub\SoftwareEngineeringGroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00290732\Documents\GitHub\SoftwareEngineeringGroup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B00E56-BF53-4D0C-903B-FD871AC5E61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCC572F-4E11-4DBB-99CB-A9B514B143BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9D383CA2-141C-48A3-B072-019372FD3699}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{9D383CA2-141C-48A3-B072-019372FD3699}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
     <sheet name="Delivery Driver" sheetId="2" r:id="rId2"/>
+    <sheet name="Delivery Docket" sheetId="3" r:id="rId3"/>
+    <sheet name="Newsagent" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>Number</t>
   </si>
@@ -344,13 +346,19 @@
   </si>
   <si>
     <t>Verify valid end date is not before start date</t>
+  </si>
+  <si>
+    <t>I want to create a delivery docket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">so that </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +424,13 @@
       <name val="Aptos Narrow"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -455,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -481,6 +496,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,19 +836,19 @@
   </sheetPr>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" customWidth="1"/>
-    <col min="2" max="2" width="62.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="76.36328125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="62.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="76.375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,12 +859,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -859,7 +875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -867,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -875,12 +891,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -891,7 +907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -899,7 +915,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
@@ -907,10 +923,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -921,7 +937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -929,16 +945,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -949,7 +965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="B22" s="2" t="s">
         <v>15</v>
       </c>
@@ -957,12 +973,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -973,7 +989,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="B26" s="2" t="s">
         <v>87</v>
       </c>
@@ -981,7 +997,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="B27" s="2" t="s">
         <v>88</v>
       </c>
@@ -989,17 +1005,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="C28" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3">
       <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>6</v>
       </c>
@@ -1010,7 +1026,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3">
       <c r="B33" s="2" t="s">
         <v>89</v>
       </c>
@@ -1018,7 +1034,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3">
       <c r="B34" s="2" t="s">
         <v>90</v>
       </c>
@@ -1026,7 +1042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>7</v>
       </c>
@@ -1037,7 +1053,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3">
       <c r="B37" s="2" t="s">
         <v>91</v>
       </c>
@@ -1045,7 +1061,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3">
       <c r="B38" s="2" t="s">
         <v>93</v>
       </c>
@@ -1053,7 +1069,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>8</v>
       </c>
@@ -1064,7 +1080,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3">
       <c r="B42" s="2" t="s">
         <v>94</v>
       </c>
@@ -1072,7 +1088,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3">
       <c r="B43" s="2" t="s">
         <v>95</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>9</v>
       </c>
@@ -1091,7 +1107,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3">
       <c r="B51" s="2" t="s">
         <v>82</v>
       </c>
@@ -1099,7 +1115,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3">
       <c r="B52" s="2" t="s">
         <v>96</v>
       </c>
@@ -1107,12 +1123,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3">
       <c r="C53" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3">
       <c r="A55" s="1">
         <v>10</v>
       </c>
@@ -1123,7 +1139,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3">
       <c r="B56" s="2" t="s">
         <v>99</v>
       </c>
@@ -1131,7 +1147,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3">
       <c r="B57" s="2" t="s">
         <v>97</v>
       </c>
@@ -1139,7 +1155,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3">
       <c r="A59" s="1">
         <v>11</v>
       </c>
@@ -1151,17 +1167,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CCE5AA-B39A-4152-A321-5C00D3D671A4}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.34998626667073579"/>
+  </sheetPr>
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="78.453125" customWidth="1"/>
-    <col min="3" max="3" width="85.453125" customWidth="1"/>
+    <col min="2" max="2" width="78.5" customWidth="1"/>
+    <col min="3" max="3" width="85.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1172,7 +1193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1183,7 +1204,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15">
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
@@ -1191,7 +1212,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15">
       <c r="B5" s="2" t="s">
         <v>67</v>
       </c>
@@ -1199,22 +1220,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15">
       <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15">
       <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="15">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" s="12">
         <v>2</v>
       </c>
@@ -1225,7 +1246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15">
       <c r="B10" s="2" t="s">
         <v>49</v>
       </c>
@@ -1233,15 +1254,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="15">
       <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="15">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="15">
       <c r="A13" s="12">
         <v>3</v>
       </c>
@@ -1252,7 +1273,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="15">
       <c r="B14" s="2" t="s">
         <v>51</v>
       </c>
@@ -1260,15 +1281,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="15">
       <c r="B15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="12">
         <v>4</v>
       </c>
@@ -1279,7 +1300,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="15">
       <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
@@ -1287,15 +1308,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="15">
       <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="15">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="8">
         <v>5</v>
       </c>
@@ -1306,7 +1327,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="15">
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1314,7 +1335,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="15">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1322,34 +1343,34 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="15">
       <c r="B24" s="2"/>
       <c r="C24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="15">
       <c r="B25" s="2"/>
       <c r="C25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="C26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="C27" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="C28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" s="8">
         <v>6</v>
       </c>
@@ -1360,7 +1381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15">
       <c r="B31" s="2" t="s">
         <v>36</v>
       </c>
@@ -1368,7 +1389,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="15">
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1376,19 +1397,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15">
       <c r="B33" s="2"/>
       <c r="C33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15">
       <c r="B34" s="2"/>
       <c r="C34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="15">
       <c r="A36" s="9">
         <v>7</v>
       </c>
@@ -1399,7 +1420,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="15">
       <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
@@ -1407,12 +1428,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="15">
       <c r="B38" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="15">
       <c r="A40" s="9">
         <v>8</v>
       </c>
@@ -1423,7 +1444,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="15">
       <c r="B41" s="2" t="s">
         <v>44</v>
       </c>
@@ -1431,7 +1452,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="15">
       <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
@@ -1439,37 +1460,37 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="15">
       <c r="B43" s="2"/>
       <c r="C43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="15">
       <c r="B44" s="2"/>
       <c r="C44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="15">
       <c r="B45" s="2"/>
       <c r="C45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="15">
       <c r="B46" s="2"/>
       <c r="C46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="15">
       <c r="B47" s="2"/>
       <c r="C47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="15">
       <c r="A49" s="9">
         <v>9</v>
       </c>
@@ -1480,7 +1501,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="15">
       <c r="B50" s="2" t="s">
         <v>60</v>
       </c>
@@ -1488,7 +1509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="15">
       <c r="B51" s="2" t="s">
         <v>61</v>
       </c>
@@ -1496,7 +1517,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="15">
       <c r="A53" s="9">
         <v>10</v>
       </c>
@@ -1507,7 +1528,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="15">
       <c r="B54" s="2" t="s">
         <v>75</v>
       </c>
@@ -1515,7 +1536,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="15">
       <c r="B55" s="2" t="s">
         <v>76</v>
       </c>
@@ -1523,31 +1544,86 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="15">
       <c r="B56" s="2"/>
       <c r="C56" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="15">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="15">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="15">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="15">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="15">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="15">
       <c r="B62" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388B29F0-9C74-42C7-87F6-AEC755062614}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="B1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="35.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="54.75" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
+      <c r="B2" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5938CEC-1BD4-42F5-AC57-0BB3D1109D0C}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>